<commit_message>
The basic flow of the program has been set, and the instructions have been updated to reflect how it works.
</commit_message>
<xml_diff>
--- a/Spreadsheet.xlsx
+++ b/Spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://partnershealthcare-my.sharepoint.com/personal/dsorkhab_mgh_harvard_edu/Documents/ONEDRIVE DOCUMENTS/CODE/Annual-Bulk-Emailer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="44" documentId="13_ncr:1_{090FF93C-DE3C-4229-AAD4-561A4201EF82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{15ACB766-2357-4E13-ADDC-3AF8ECBFF878}"/>
+  <xr:revisionPtr revIDLastSave="53" documentId="13_ncr:1_{090FF93C-DE3C-4229-AAD4-561A4201EF82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4C7D30EB-DC47-4C40-B4C5-4F2390DE65D1}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{C3C2520B-3B09-45AE-AD06-18BFA46C4AC0}"/>
   </bookViews>
@@ -36,8 +36,49 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Sorkhab, Drake Liu</author>
+  </authors>
+  <commentList>
+    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{23D8DC53-6AA1-4E1E-AEC5-438433050507}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Sorkhab, Drake Liu:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+This is done automatically by the program.
+Examples:
+"Previously emailed on 12/22/2023."
+"Previous emailed on 12/22/2023. Previously emailed on 12/25/2023."
+"Document for 2023 received and awaiting printing."
+"Document for 2023 printed and awaiting upload."
+"Document for 2023 uploaded."
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="25">
   <si>
     <t>Code Red Drill</t>
   </si>
@@ -106,13 +147,19 @@
   </si>
   <si>
     <t>Washington Carver(did I email her? Im tl n sure)</t>
+  </si>
+  <si>
+    <t>OFFICE/RECIPIENT TITLE</t>
+  </si>
+  <si>
+    <t>Status (usually auto-entered)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -201,6 +248,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -607,11 +667,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{578FFF7B-6B52-4AC7-A90A-177440216DE7}">
-  <dimension ref="A1:I280"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{578FFF7B-6B52-4AC7-A90A-177440216DE7}">
+  <dimension ref="A1:H280"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1130,11 +1190,11 @@
     <col min="16136" max="16136" width="32" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="3"/>
       <c r="B1" s="3"/>
       <c r="C1" s="4" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>7</v>
@@ -1148,10 +1208,11 @@
       <c r="G1" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
+      <c r="H1" s="16" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="1" t="s">
@@ -1167,9 +1228,8 @@
         <v>17</v>
       </c>
       <c r="H2" s="17"/>
-      <c r="I2" s="12"/>
     </row>
-    <row r="3" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="1" t="s">
@@ -1185,9 +1245,8 @@
         <v>18</v>
       </c>
       <c r="H3" s="17"/>
-      <c r="I3" s="12"/>
     </row>
-    <row r="4" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="1" t="s">
@@ -1203,9 +1262,8 @@
         <v>19</v>
       </c>
       <c r="H4" s="17"/>
-      <c r="I4" s="12"/>
     </row>
-    <row r="5" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="1" t="s">
@@ -1221,9 +1279,8 @@
         <v>5</v>
       </c>
       <c r="H5" s="17"/>
-      <c r="I5" s="12"/>
     </row>
-    <row r="6" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="1" t="s">
@@ -1235,9 +1292,8 @@
         <v>20</v>
       </c>
       <c r="H6" s="17"/>
-      <c r="I6" s="12"/>
     </row>
-    <row r="7" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="1" t="s">
@@ -1254,7 +1310,7 @@
       </c>
       <c r="H7" s="17"/>
     </row>
-    <row r="8" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="1" t="s">
@@ -1268,7 +1324,6 @@
         <v>22</v>
       </c>
       <c r="H8" s="17"/>
-      <c r="I8" s="12"/>
     </row>
     <row r="24" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="28" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2"/>
@@ -1283,6 +1338,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1976,17 +2032,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="09ac68c9-e146-4d51-a650-c6d16a715f98">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="d1680238-2266-4ab1-9ebd-8eb4f05a8cbc" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000C5C42DE853CEF408AEE3884C4101B5F" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5ae15d59986d80c154e1603f957e677a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="09ac68c9-e146-4d51-a650-c6d16a715f98" xmlns:ns3="d1680238-2266-4ab1-9ebd-8eb4f05a8cbc" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1a0899c497c6ed3c7dad0375e58f3f38" ns2:_="" ns3:_="">
     <xsd:import namespace="09ac68c9-e146-4d51-a650-c6d16a715f98"/>
@@ -2181,6 +2226,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="09ac68c9-e146-4d51-a650-c6d16a715f98">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="d1680238-2266-4ab1-9ebd-8eb4f05a8cbc" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62DF1655-C6F2-4874-B5B4-E8E17737874D}">
   <ds:schemaRefs>
@@ -2190,23 +2246,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{79A966C1-B130-43CB-9C5B-FC60018CB7DE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="09ac68c9-e146-4d51-a650-c6d16a715f98"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="d1680238-2266-4ab1-9ebd-8eb4f05a8cbc"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AD3E7137-47EF-4FFF-B240-CF30B9AAB00E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2223,4 +2262,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{79A966C1-B130-43CB-9C5B-FC60018CB7DE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="09ac68c9-e146-4d51-a650-c6d16a715f98"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="d1680238-2266-4ab1-9ebd-8eb4f05a8cbc"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>